<commit_message>
Avanços feitos em Aula
</commit_message>
<xml_diff>
--- a/Matriz de Rastreabilidade dos Requisitos - Felipe e Ryan.xlsx
+++ b/Matriz de Rastreabilidade dos Requisitos - Felipe e Ryan.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20380"/>
   <workbookPr defaultThemeVersion="123820"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dti\Desktop\Engenharia_SW_Felipe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dti\Desktop\Exercícios_Satoshi\Documentacao_Exercicio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34FC01F3-4A33-4FAE-92ED-FDDB45A5B91E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BE7CD0-999A-48AD-86CC-F50DF9D1F691}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requisitos" sheetId="7" r:id="rId1"/>
-    <sheet name="Planilha1" sheetId="10" r:id="rId2"/>
-    <sheet name="Param" sheetId="9" r:id="rId3"/>
+    <sheet name="Param" sheetId="9" r:id="rId2"/>
+    <sheet name="Padaria" sheetId="10" r:id="rId3"/>
+    <sheet name="Buffet" sheetId="11" r:id="rId4"/>
+    <sheet name="Clube Cultural" sheetId="12" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Prioridade">Param!$C$4:$C$11</definedName>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="200">
   <si>
     <t>Prioridade</t>
   </si>
@@ -306,9 +308,6 @@
     <t>Cadastro de produtos</t>
   </si>
   <si>
-    <t>Os produtos que constituem o cardápio devem ser cadastrado previamente pelos colaboradores da padaria, para serem exibidos.</t>
-  </si>
-  <si>
     <t>Seu Joaquim</t>
   </si>
   <si>
@@ -360,25 +359,277 @@
     <t>Criar numeração automática para identificação única da comanda de venda.</t>
   </si>
   <si>
-    <t>Calcular valores gastos</t>
-  </si>
-  <si>
-    <t>Calcular todos os valores unitários consumidos e totalizá-los.</t>
-  </si>
-  <si>
     <t>RF09</t>
   </si>
   <si>
     <t>RF10</t>
   </si>
   <si>
-    <t>Geração de relatórios</t>
-  </si>
-  <si>
-    <t>Criação de relatórios descrevendo a situação graficamente dos setores de venda, estoque e produto.</t>
-  </si>
-  <si>
-    <t>Pagar por PIX, Cartão de Crédito ou débito</t>
+    <t>Pagar por PIX, Cartão de Crédito ou débito e dinheiro</t>
+  </si>
+  <si>
+    <t>Realização de backup</t>
+  </si>
+  <si>
+    <t>Multiplataforma</t>
+  </si>
+  <si>
+    <t>Acesso em diferentes sistemas operacionais</t>
+  </si>
+  <si>
+    <t>Fluxo de processos</t>
+  </si>
+  <si>
+    <t>Organização sequencial de processos para feitos para concluir uma tarefa.</t>
+  </si>
+  <si>
+    <t>Guia de estilos do sistema</t>
+  </si>
+  <si>
+    <t>Padronização do estilo do site, seguindo as mesmas cor, tipografia, espaçamento e formatos.</t>
+  </si>
+  <si>
+    <t>RNF06</t>
+  </si>
+  <si>
+    <t>Banco de dados relacional</t>
+  </si>
+  <si>
+    <t>As informações armazenadas no banco de dados terão um relacionamento entre elas.</t>
+  </si>
+  <si>
+    <t>RNF07</t>
+  </si>
+  <si>
+    <t>RNF08</t>
+  </si>
+  <si>
+    <t>RNF09</t>
+  </si>
+  <si>
+    <t>Carregar entrada de estoque por XML</t>
+  </si>
+  <si>
+    <t>Demonstrar estrutura de preços na comanda</t>
+  </si>
+  <si>
+    <t>Os dados referentes ao estoque serão gravados no XML, possibilitando maior possibilidade de armazenamento de dados no Excel.</t>
+  </si>
+  <si>
+    <t>Demonstrar todos os valores unitários, suas quantidade e somatória de todos os valores. Apresentando o resultado para o usuário</t>
+  </si>
+  <si>
+    <t>Cadastro dos clientes</t>
+  </si>
+  <si>
+    <t>Cadastro de tema</t>
+  </si>
+  <si>
+    <t>Cadastrar os dados pessoais do cliente e suas ações dentro do aplicação de software.</t>
+  </si>
+  <si>
+    <t>Mostra os temas de buffet disponíveis para festas infantis de aluguel.</t>
+  </si>
+  <si>
+    <t>Sistema de cálculo de orçamento</t>
+  </si>
+  <si>
+    <t>Tendo em base o tema da festa junina, os serviços prestados e descontos que dependem do cliente.</t>
+  </si>
+  <si>
+    <t>Verificação de cliente que contém desconto</t>
+  </si>
+  <si>
+    <t>Verificação se há clientes antigos para aplicar-lhes descontos.</t>
+  </si>
+  <si>
+    <t>Agenda de cronogramas dos locais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agendamento de cada serviço que será prestado e o seu local. </t>
+  </si>
+  <si>
+    <t>Geração do valor total</t>
+  </si>
+  <si>
+    <t>Calcular todos os serviços e produtos vendidos, deslocamento e tema, para basear-se no cálculo final.</t>
+  </si>
+  <si>
+    <t>Indicar no sistema quais são as funções designadas para cada pessoa realizar.</t>
+  </si>
+  <si>
+    <t>Distribuição das ordens de serviço e produtos para os funcionários</t>
+  </si>
+  <si>
+    <t>Manual técnico dos produtos para cada tema</t>
+  </si>
+  <si>
+    <t>Cada tema possui uma especificação de tarefas para serem realizadas.</t>
+  </si>
+  <si>
+    <t>Diferentes formas de se pagar a conta gerada</t>
+  </si>
+  <si>
+    <t>Gerenciamento de logística</t>
+  </si>
+  <si>
+    <t>Organizar os tempos e horários para não ocorrem colisões</t>
+  </si>
+  <si>
+    <t>Pagar à vista e à prazo</t>
+  </si>
+  <si>
+    <t>Possibilitar a fatoração do prazo de pagamento ou o pagamento de todo o preço</t>
+  </si>
+  <si>
+    <t>Pagar no Boleto PagSeguro, Cartão de Crédito e Débito, PIX e Paypal</t>
+  </si>
+  <si>
+    <t>Van para efetuar as entregas</t>
+  </si>
+  <si>
+    <t>Utilização de vans para poderem transportar os alimentos até o local da festa.</t>
+  </si>
+  <si>
+    <t>Possibilização de escolha da forma de pagamento</t>
+  </si>
+  <si>
+    <t>Status de confirmação do Buffet</t>
+  </si>
+  <si>
+    <t>Buffet deve indicar no sistema que a entrega será feita.</t>
+  </si>
+  <si>
+    <t>Cadastrar a coleção de revistas em quadrinho</t>
+  </si>
+  <si>
+    <t>Avaliar a condição das revistas</t>
+  </si>
+  <si>
+    <t>Checagem das coleções de revistas após uso dos amiguinhos.</t>
+  </si>
+  <si>
+    <t>As coleções deverão ser cadastradas pelo administradores ou moderadores. No cadastro deve ter: tipo da coleção, número da edição, ano da revista e caixa onde está.</t>
+  </si>
+  <si>
+    <t>Classificar os quadrinhos por tipo de coleção</t>
+  </si>
+  <si>
+    <t>Agrupar os quadrinhos conforme os seus tipos</t>
+  </si>
+  <si>
+    <t>Controle de empréstimos</t>
+  </si>
+  <si>
+    <t>Com a data de devolução é possível controlar se a coleção de revistas existe no clube e quando retornará.</t>
+  </si>
+  <si>
+    <t>Cadastro de amigos que pegaram revistas emprestadas</t>
+  </si>
+  <si>
+    <t>Cadastro dos amiguinhos para possíveis contatos e onde mora</t>
+  </si>
+  <si>
+    <t>Ian</t>
+  </si>
+  <si>
+    <t>Visualização do histórico de solicitações dos quadrinhos</t>
+  </si>
+  <si>
+    <t>Mostra o histórico de empréstimos feitos para a coleção de quadrinho</t>
+  </si>
+  <si>
+    <t>Seção de comentários da revista</t>
+  </si>
+  <si>
+    <t>Comentários deixados pelos usuários que leram as revistas em quadrinhos</t>
+  </si>
+  <si>
+    <t>Verificação de atrasos dos empréstimos</t>
+  </si>
+  <si>
+    <t>Controle de atrasos dos empréstimos e as pessoas que cometeram o atraso</t>
+  </si>
+  <si>
+    <t>Inventário das revistas</t>
+  </si>
+  <si>
+    <t>Revistas que estão presentes no clube cultural</t>
+  </si>
+  <si>
+    <t>Cadastro das caixas</t>
+  </si>
+  <si>
+    <t>Cadastra-se a cor, uma etiqueta e um número; para localização das revistas em quadrinhos.</t>
+  </si>
+  <si>
+    <t>Mandar um alerta vermelho na finalização do projeto</t>
+  </si>
+  <si>
+    <t>Quando faltar 1 dia para acabar a data de devolução irá alertar no sistema do administrador sobre o empréstimo e sua data de devolução</t>
+  </si>
+  <si>
+    <t>Avaliar revistas em até 5 estrelas</t>
+  </si>
+  <si>
+    <t>Mensuração de qualidade do conteúdo da coleção de quadrinhos</t>
+  </si>
+  <si>
+    <t>Informar o status do empréstimo no histórico</t>
+  </si>
+  <si>
+    <t>Informar a situação atual do empréstimo: já foi entregue, atrasado, perto de ser entregue e emprestado.</t>
+  </si>
+  <si>
+    <t>Consultas devem ser possíveis e exibidas as informações pesquisadas</t>
+  </si>
+  <si>
+    <t>As possibilidades de pagamento devem ser apresentadas na comanda e efetuada a transação econômica</t>
+  </si>
+  <si>
+    <t>O sistema deverá ser adaptável a diferentes sistemas operacionais</t>
+  </si>
+  <si>
+    <t>Os dados no banco de dados devem ser gravados ao final do dia</t>
+  </si>
+  <si>
+    <t>Cálculo das comandas</t>
+  </si>
+  <si>
+    <t>O cálculo é dado pela fórmula: (QtdProdutos * valor)  + (QtdProdutos * valor)</t>
+  </si>
+  <si>
+    <t>Cálculo para finalização das comandas</t>
+  </si>
+  <si>
+    <t>Condição para saída do estabelecimento</t>
+  </si>
+  <si>
+    <t>Condicional de finalização do processo</t>
+  </si>
+  <si>
+    <t>Caso cliente pague a comanda, poderá sair do estabelecimento</t>
+  </si>
+  <si>
+    <t>Sequência lógica deve ser imposta pelo administrador e testada em produção</t>
+  </si>
+  <si>
+    <t>Status da NFC-E</t>
+  </si>
+  <si>
+    <t>Gerada uma nota fiscal na finalização do pedido</t>
+  </si>
+  <si>
+    <t>O sistema deverá gerar uma nota fiscal eletrônica para toda comanda paga.</t>
+  </si>
+  <si>
+    <t>O sistema deverá disponibilizar e gravar as informações no banco de dados referente ao estoque.</t>
+  </si>
+  <si>
+    <t>O sistema na geração de comandas irá apresentar as informações listadas</t>
+  </si>
+  <si>
+    <t>Os produtos irão apresentar suas imagens, nome, ingredientes e número do código.</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1255,7 @@
     <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
@@ -1052,6 +1303,9 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="36" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="37" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="46">
@@ -1102,7 +1356,37 @@
     <cellStyle name="Título 4" xfId="35" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -1486,8 +1770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J30"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1882,7 +2166,7 @@
         <v>43763</v>
       </c>
     </row>
-    <row r="15" spans="2:10" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B15" s="22" t="s">
         <v>74</v>
       </c>
@@ -2062,27 +2346,27 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <conditionalFormatting sqref="I3:I15">
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2109,11 +2393,169 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B2:G12"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="18"/>
+      <c r="G2" s="19"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="20"/>
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="13"/>
+      <c r="C5" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="20"/>
+      <c r="G5" s="21"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="13"/>
+      <c r="C6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="21"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="13"/>
+      <c r="C7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="20"/>
+      <c r="G7" s="21"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="13"/>
+      <c r="C8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="13"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="15"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;LMatriz de rastreabilidade dos requisitos&amp;R&amp;A</oddHeader>
+    <oddFooter>&amp;LPMO Escritório de Projetos LTDA
+&amp;F&amp;RPágina &amp;P de &amp;N
+http://escritoriodeprojetos.com.br</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48FADF18-2922-42A8-B41A-69F9B4DDFDBE}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2169,7 +2611,7 @@
         <v>91</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>92</v>
+        <v>199</v>
       </c>
       <c r="E2" s="23" t="s">
         <v>26</v>
@@ -2178,13 +2620,13 @@
         <v>16</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="I2" s="24">
-        <v>44650</v>
+        <v>44622</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.2">
@@ -2195,25 +2637,25 @@
         <v>25</v>
       </c>
       <c r="C3" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="E3" s="23" t="s">
         <v>95</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>96</v>
       </c>
       <c r="F3" s="22" t="s">
         <v>16</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="I3" s="24">
-        <v>44650</v>
+        <v>44626</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.2">
@@ -2224,25 +2666,25 @@
         <v>12</v>
       </c>
       <c r="C4" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="E4" s="23" t="s">
         <v>98</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>99</v>
       </c>
       <c r="F4" s="22" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I4" s="24">
-        <v>44657</v>
+        <v>44628</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.2">
@@ -2253,10 +2695,10 @@
         <v>25</v>
       </c>
       <c r="C5" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>100</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>101</v>
       </c>
       <c r="E5" s="23" t="s">
         <v>40</v>
@@ -2265,7 +2707,7 @@
         <v>16</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H5" s="22" t="s">
         <v>9</v>
@@ -2282,19 +2724,19 @@
         <v>10</v>
       </c>
       <c r="C6" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>103</v>
-      </c>
       <c r="E6" s="23" t="s">
-        <v>26</v>
+        <v>183</v>
       </c>
       <c r="F6" s="22" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H6" s="22" t="s">
         <v>11</v>
@@ -2303,7 +2745,7 @@
         <v>43756</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>67</v>
       </c>
@@ -2311,19 +2753,19 @@
         <v>10</v>
       </c>
       <c r="C7" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="23" t="s">
-        <v>105</v>
-      </c>
       <c r="E7" s="23" t="s">
-        <v>40</v>
+        <v>184</v>
       </c>
       <c r="F7" s="22" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H7" s="22" t="s">
         <v>9</v>
@@ -2340,10 +2782,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="23" t="s">
         <v>106</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>107</v>
       </c>
       <c r="E8" s="23" t="s">
         <v>44</v>
@@ -2352,7 +2794,7 @@
         <v>16</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H8" s="22" t="s">
         <v>9</v>
@@ -2369,10 +2811,10 @@
         <v>25</v>
       </c>
       <c r="C9" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="23" t="s">
         <v>108</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>109</v>
       </c>
       <c r="E9" s="23" t="s">
         <v>47</v>
@@ -2381,7 +2823,7 @@
         <v>16</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H9" s="22" t="s">
         <v>9</v>
@@ -2390,121 +2832,123 @@
         <v>43759</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
-        <v>112</v>
+        <v>70</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>110</v>
+        <v>12</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>111</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>111</v>
+        <v>54</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="F10" s="23" t="s">
         <v>49</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H10" s="22" t="s">
         <v>9</v>
       </c>
       <c r="I10" s="24">
-        <v>43760</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="90" x14ac:dyDescent="0.2">
+        <v>43762</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
-        <v>113</v>
+        <v>71</v>
       </c>
       <c r="B11" s="22" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>52</v>
+        <v>186</v>
       </c>
       <c r="F11" s="23" t="s">
         <v>49</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H11" s="22" t="s">
         <v>9</v>
       </c>
       <c r="I11" s="24">
-        <v>43761</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+        <v>43763</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="22"/>
+      <c r="G12" s="22" t="s">
+        <v>92</v>
+      </c>
       <c r="H12" s="22" t="s">
         <v>9</v>
       </c>
       <c r="I12" s="24">
-        <v>43762</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="225" x14ac:dyDescent="0.2">
+        <v>44646</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
         <v>73</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>56</v>
+        <v>10</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>115</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>57</v>
+        <v>116</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>58</v>
+        <v>193</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>49</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="H13" s="22" t="s">
         <v>9</v>
       </c>
       <c r="I13" s="24">
-        <v>43763</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="225" x14ac:dyDescent="0.2">
+        <v>44646</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
         <v>74</v>
       </c>
@@ -2512,48 +2956,46 @@
         <v>8</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>59</v>
+        <v>120</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>61</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="E14" s="23"/>
       <c r="F14" s="23" t="s">
         <v>49</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="H14" s="22" t="s">
         <v>9</v>
       </c>
       <c r="I14" s="24">
-        <v>43764</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="165" x14ac:dyDescent="0.2">
+        <v>44652</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>80</v>
+        <v>117</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>76</v>
+        <v>118</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>77</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="G15" s="22" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="H15" s="22" t="s">
         <v>11</v>
@@ -2562,100 +3004,1279 @@
         <v>43764</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="105" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>85</v>
+        <v>8</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>80</v>
+        <v>194</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>76</v>
+        <v>195</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>81</v>
+        <v>196</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="I16" s="24">
-        <v>43764</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="150" x14ac:dyDescent="0.2">
+        <v>44623</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="75" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>86</v>
+        <v>6</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>76</v>
+        <v>127</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>83</v>
+        <v>197</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="H17" s="22" t="s">
         <v>11</v>
       </c>
       <c r="I17" s="24">
-        <v>43764</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="150" x14ac:dyDescent="0.2">
+        <v>44648</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="B18" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="24">
+        <v>44617</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+      <c r="A19" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18" s="23" t="s">
+      <c r="C19" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="F19" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="G18" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="H18" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" s="24">
-        <v>43764</v>
+      <c r="G19" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="24">
+        <v>44622</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+      <c r="A20" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="24">
+        <v>44666</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H2:H14">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+  <conditionalFormatting sqref="H20 H2:H14 H16:H18">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H20" xr:uid="{ACFBE0EA-6BDE-4487-BE4E-D36A79555177}">
+      <formula1>Status</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F20" xr:uid="{FA23D74C-1A06-482F-84B2-91A33ECB30D9}">
+      <formula1>Tipo</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B20" xr:uid="{130B2BB6-BD83-4D5B-9005-BD413173ADEB}">
+      <formula1>Prioridade</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BADEEDB-A139-492C-9ABF-B310E3BC3E8A}">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A1" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="26">
+        <v>44650</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="26">
+        <v>44650</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="26">
+        <v>44657</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="26">
+        <v>44659</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="26">
+        <v>43756</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="26">
+        <v>43757</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="26">
+        <v>43758</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="26">
+        <v>43759</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+      <c r="A10" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="26">
+        <v>43760</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="90" x14ac:dyDescent="0.2">
+      <c r="A11" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="26">
+        <v>43761</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+      <c r="A12" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="26">
+        <v>43762</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+      <c r="A13" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="26">
+        <v>43763</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+      <c r="A14" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="26">
+        <v>43764</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A15" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="26"/>
+    </row>
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="26">
+        <v>43764</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+      <c r="A17" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="26">
+        <v>43764</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+      <c r="A18" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="26">
+        <v>43764</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="H2:H15">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B18" xr:uid="{8BFD2F1D-4F26-43FE-9229-40BC5D9D395A}">
+      <formula1>Prioridade</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F18" xr:uid="{02D473B4-757A-493E-AED2-B0093A0F8807}">
+      <formula1>Tipo</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H18" xr:uid="{BB0F10A6-15FA-47D0-85ED-7B43B0D8940C}">
+      <formula1>Status</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40FB3C50-76AA-4A99-994A-634E15544F82}">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="26">
+        <v>44650</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="26">
+        <v>44650</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="26">
+        <v>44657</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="26">
+        <v>44659</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="26">
+        <v>43756</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="26">
+        <v>43757</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="26">
+        <v>43758</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="26">
+        <v>43759</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+      <c r="A10" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="26">
+        <v>43760</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+      <c r="A11" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="26">
+        <v>43761</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.2">
+      <c r="A12" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="26">
+        <v>43762</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+      <c r="A13" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="26">
+        <v>43763</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+      <c r="A14" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="26">
+        <v>43764</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+      <c r="A15" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="26"/>
+    </row>
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="26">
+        <v>43764</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+      <c r="A17" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="26">
+        <v>43764</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+      <c r="A18" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="26">
+        <v>43764</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="H2:H15">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -2676,174 +4297,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H18" xr:uid="{ACFBE0EA-6BDE-4487-BE4E-D36A79555177}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H18" xr:uid="{FB4F3762-8BAE-40AD-A5D3-27DC6E9744E7}">
       <formula1>Status</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F18" xr:uid="{FA23D74C-1A06-482F-84B2-91A33ECB30D9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F18" xr:uid="{12E8D30E-24EC-438A-A3FB-6E1E97E0E190}">
       <formula1>Tipo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B18" xr:uid="{130B2BB6-BD83-4D5B-9005-BD413173ADEB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B18" xr:uid="{5975023F-0645-4063-8320-EE3589AC700A}">
       <formula1>Prioridade</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:G12"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="19"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="21"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="13"/>
-      <c r="C5" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="13"/>
-      <c r="C6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="13"/>
-      <c r="C7" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
-      <c r="C8" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="21"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
-  <headerFooter alignWithMargins="0">
-    <oddHeader>&amp;LMatriz de rastreabilidade dos requisitos&amp;R&amp;A</oddHeader>
-    <oddFooter>&amp;LPMO Escritório de Projetos LTDA
-&amp;F&amp;RPágina &amp;P de &amp;N
-http://escritoriodeprojetos.com.br</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Caso de uso - Clube Cultural
</commit_message>
<xml_diff>
--- a/Matriz de Rastreabilidade dos Requisitos - Felipe e Ryan.xlsx
+++ b/Matriz de Rastreabilidade dos Requisitos - Felipe e Ryan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dti\Desktop\SatoshiAtividae\Documentacao_Exercicio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AF82DD-1885-4882-AB43-DEC9AD9D1B46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82DBB97-65DC-45AC-91D4-CA2521E9E975}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exemplo Satochi" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="203">
   <si>
     <t>Prioridade</t>
   </si>
@@ -1365,22 +1365,7 @@
     <cellStyle name="Título 4" xfId="35" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <color theme="0"/>
@@ -2131,7 +2116,7 @@
         <v>43762</v>
       </c>
     </row>
-    <row r="14" spans="2:10" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="22" t="s">
         <v>73</v>
       </c>
@@ -2160,7 +2145,7 @@
         <v>43763</v>
       </c>
     </row>
-    <row r="15" spans="2:10" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B15" s="22" t="s">
         <v>74</v>
       </c>
@@ -2340,27 +2325,27 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <conditionalFormatting sqref="I3:I15">
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17">
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3146,17 +3131,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I21 I3:I15 I17:I19">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3179,8 +3164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BADEEDB-A139-492C-9ABF-B310E3BC3E8A}">
   <dimension ref="B2:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3224,7 +3209,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="75" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" ht="45" x14ac:dyDescent="0.2">
       <c r="B3" s="23" t="s">
         <v>62</v>
       </c>
@@ -3253,7 +3238,7 @@
         <v>44650</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="75" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" ht="45" x14ac:dyDescent="0.2">
       <c r="B4" s="23" t="s">
         <v>63</v>
       </c>
@@ -3282,7 +3267,7 @@
         <v>44650</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="90" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" ht="60" x14ac:dyDescent="0.2">
       <c r="B5" s="23" t="s">
         <v>64</v>
       </c>
@@ -3311,7 +3296,7 @@
         <v>44657</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="60" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10" ht="45" x14ac:dyDescent="0.2">
       <c r="B6" s="23" t="s">
         <v>65</v>
       </c>
@@ -3340,7 +3325,7 @@
         <v>44659</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="60" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" ht="45" x14ac:dyDescent="0.2">
       <c r="B7" s="23" t="s">
         <v>66</v>
       </c>
@@ -3427,7 +3412,7 @@
         <v>43758</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="75" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" ht="45" x14ac:dyDescent="0.2">
       <c r="B10" s="23" t="s">
         <v>69</v>
       </c>
@@ -3485,7 +3470,7 @@
         <v>43760</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="90" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" ht="45" x14ac:dyDescent="0.2">
       <c r="B12" s="23" t="s">
         <v>110</v>
       </c>
@@ -3572,7 +3557,7 @@
         <v>43763</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="75" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" ht="45" x14ac:dyDescent="0.2">
       <c r="B15" s="23" t="s">
         <v>72</v>
       </c>
@@ -3632,7 +3617,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I3:I16">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3653,10 +3638,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40FB3C50-76AA-4A99-994A-634E15544F82}">
-  <dimension ref="B2:J19"/>
+  <dimension ref="B2:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4078,143 +4063,20 @@
         <v>43764</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="45" x14ac:dyDescent="0.2">
-      <c r="B16" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="I16" s="23"/>
-      <c r="J16" s="26"/>
-    </row>
-    <row r="17" spans="2:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="B17" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="G17" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="H17" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="I17" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="J17" s="26">
-        <v>43764</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="45" x14ac:dyDescent="0.2">
-      <c r="B18" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G18" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="H18" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="I18" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" s="26">
-        <v>43764</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="45" x14ac:dyDescent="0.2">
-      <c r="B19" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="G19" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="H19" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="I19" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="J19" s="26">
-        <v>43764</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="I3:I16">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I19">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="I3:I15">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I19" xr:uid="{FB4F3762-8BAE-40AD-A5D3-27DC6E9744E7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I15" xr:uid="{FB4F3762-8BAE-40AD-A5D3-27DC6E9744E7}">
       <formula1>Status</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G19" xr:uid="{12E8D30E-24EC-438A-A3FB-6E1E97E0E190}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G15" xr:uid="{12E8D30E-24EC-438A-A3FB-6E1E97E0E190}">
       <formula1>Tipo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C19" xr:uid="{5975023F-0645-4063-8320-EE3589AC700A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C15" xr:uid="{5975023F-0645-4063-8320-EE3589AC700A}">
       <formula1>Prioridade</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>